<commit_message>
Loose Coupling - Reflection concept
</commit_message>
<xml_diff>
--- a/Test Data/LoginPage.xlsx
+++ b/Test Data/LoginPage.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mani3359\Downloads\RFW-Practice\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863A4D30-285B-4ECE-9E13-69765C3DC2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2121ED2-6988-4679-B43D-E9E8DE1BAD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Negative Scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="Positive Scenario" sheetId="2" r:id="rId2"/>
+    <sheet name="Login Scenario" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>invalid_username</t>
   </si>
@@ -38,6 +37,39 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Enter invalid username and invalid password</t>
+  </si>
+  <si>
+    <t>Enter invalid username and valid password</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Enter valid username and invalid password</t>
+  </si>
+  <si>
+    <t>Enter null username and invalid password</t>
+  </si>
+  <si>
+    <t>Enter valid username and null password</t>
+  </si>
+  <si>
+    <t>Enter null username and null password</t>
+  </si>
+  <si>
+    <t>Enter valid username and valid password</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -355,61 +387,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B3A789-37CB-4BD5-8949-BE15409757D6}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553510A6-68C8-41BC-9E5A-514E212343F2}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>